<commit_message>
changes as of 04/06/
</commit_message>
<xml_diff>
--- a/resources/ClinicianAccount.xlsx
+++ b/resources/ClinicianAccount.xlsx
@@ -54,9 +54,6 @@
     <t>input</t>
   </si>
   <si>
-    <t>clinicain</t>
-  </si>
-  <si>
     <t>Last Name</t>
   </si>
   <si>
@@ -301,6 +298,9 @@
   </si>
   <si>
     <t>//div[@class="_md-select-menu-container md-cs-content-theme-theme _md-active _md-clickable"]//md-option[9]</t>
+  </si>
+  <si>
+    <t>clinician</t>
   </si>
 </sst>
 </file>
@@ -663,7 +663,7 @@
   <dimension ref="A1:I164"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD90"/>
+      <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="15"/>
@@ -704,13 +704,13 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
         <v>37</v>
       </c>
-      <c r="B2" t="s">
-        <v>38</v>
-      </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2"/>
       <c r="E2">
@@ -727,13 +727,13 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
         <v>28</v>
       </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3"/>
       <c r="E3">
@@ -757,7 +757,7 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4"/>
       <c r="F4"/>
@@ -765,16 +765,16 @@
     </row>
     <row r="5" spans="1:9" ht="33" customHeight="1">
       <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="C5" t="s">
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E5"/>
       <c r="F5"/>
@@ -782,16 +782,16 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="C6" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E6"/>
       <c r="F6"/>
@@ -799,13 +799,13 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7"/>
       <c r="E7">
@@ -820,13 +820,13 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8"/>
       <c r="E8">
@@ -841,13 +841,13 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9"/>
       <c r="E9">
@@ -862,13 +862,13 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" t="s">
         <v>26</v>
-      </c>
-      <c r="C10" t="s">
-        <v>27</v>
       </c>
       <c r="D10"/>
       <c r="E10"/>
@@ -877,13 +877,13 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
         <v>28</v>
       </c>
-      <c r="B11" t="s">
-        <v>29</v>
-      </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D11"/>
       <c r="E11">
@@ -907,7 +907,7 @@
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>12</v>
+        <v>94</v>
       </c>
       <c r="E12"/>
       <c r="F12"/>
@@ -915,16 +915,16 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="C13" t="s">
         <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E13"/>
       <c r="F13"/>
@@ -932,16 +932,16 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
         <v>16</v>
-      </c>
-      <c r="C14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" t="s">
-        <v>17</v>
       </c>
       <c r="E14"/>
       <c r="F14"/>
@@ -949,13 +949,13 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D15"/>
       <c r="E15">
@@ -970,13 +970,13 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D16"/>
       <c r="E16">
@@ -991,13 +991,13 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17"/>
       <c r="E17">
@@ -1012,13 +1012,13 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="C18" t="s">
         <v>26</v>
-      </c>
-      <c r="C18" t="s">
-        <v>27</v>
       </c>
       <c r="D18"/>
       <c r="E18"/>
@@ -1027,13 +1027,13 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D19"/>
       <c r="E19">
@@ -1057,7 +1057,7 @@
         <v>11</v>
       </c>
       <c r="D20" t="s">
-        <v>12</v>
+        <v>94</v>
       </c>
       <c r="E20"/>
       <c r="F20"/>
@@ -1065,16 +1065,16 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="C21" t="s">
         <v>11</v>
       </c>
       <c r="D21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E21"/>
       <c r="F21"/>
@@ -1082,16 +1082,16 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="C22" t="s">
         <v>11</v>
       </c>
       <c r="D22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E22"/>
       <c r="F22"/>
@@ -1099,13 +1099,13 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="C23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D23"/>
       <c r="E23">
@@ -1120,13 +1120,13 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="C24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D24"/>
       <c r="E24">
@@ -1141,13 +1141,13 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="C25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D25"/>
       <c r="E25">
@@ -1162,13 +1162,13 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="C26" t="s">
         <v>26</v>
-      </c>
-      <c r="C26" t="s">
-        <v>27</v>
       </c>
       <c r="D26"/>
       <c r="E26"/>
@@ -1177,13 +1177,13 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="C27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D27"/>
       <c r="E27">
@@ -1207,7 +1207,7 @@
         <v>11</v>
       </c>
       <c r="D28" t="s">
-        <v>12</v>
+        <v>94</v>
       </c>
       <c r="E28"/>
       <c r="F28"/>
@@ -1215,16 +1215,16 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="C29" t="s">
         <v>11</v>
       </c>
       <c r="D29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E29"/>
       <c r="F29"/>
@@ -1232,16 +1232,16 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="C30" t="s">
         <v>11</v>
       </c>
       <c r="D30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E30"/>
       <c r="F30"/>
@@ -1249,13 +1249,13 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="C31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D31"/>
       <c r="E31">
@@ -1270,13 +1270,13 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="C32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D32"/>
       <c r="E32">
@@ -1291,13 +1291,13 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="C33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D33"/>
       <c r="E33">
@@ -1312,13 +1312,13 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="C34" t="s">
         <v>26</v>
-      </c>
-      <c r="C34" t="s">
-        <v>27</v>
       </c>
       <c r="D34"/>
       <c r="E34"/>
@@ -1327,13 +1327,13 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="C35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D35"/>
       <c r="E35">
@@ -1357,7 +1357,7 @@
         <v>11</v>
       </c>
       <c r="D36" t="s">
-        <v>12</v>
+        <v>94</v>
       </c>
       <c r="E36"/>
       <c r="F36"/>
@@ -1365,16 +1365,16 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="C37" t="s">
         <v>11</v>
       </c>
       <c r="D37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E37"/>
       <c r="F37"/>
@@ -1382,16 +1382,16 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="C38" t="s">
         <v>11</v>
       </c>
       <c r="D38" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E38"/>
       <c r="F38"/>
@@ -1399,13 +1399,13 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="C39" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D39"/>
       <c r="E39">
@@ -1420,13 +1420,13 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B40" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="C40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D40"/>
       <c r="E40">
@@ -1441,13 +1441,13 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
+        <v>22</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="C41" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D41"/>
       <c r="E41">
@@ -1462,13 +1462,13 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
+        <v>24</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="C42" t="s">
         <v>26</v>
-      </c>
-      <c r="C42" t="s">
-        <v>27</v>
       </c>
       <c r="D42"/>
       <c r="E42"/>
@@ -1477,13 +1477,13 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
+        <v>27</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B43" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="C43" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D43"/>
       <c r="E43">
@@ -1507,7 +1507,7 @@
         <v>11</v>
       </c>
       <c r="D44" t="s">
-        <v>12</v>
+        <v>94</v>
       </c>
       <c r="E44"/>
       <c r="F44"/>
@@ -1515,16 +1515,16 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="C45" t="s">
         <v>11</v>
       </c>
       <c r="D45" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E45"/>
       <c r="F45"/>
@@ -1532,16 +1532,16 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" t="s">
+        <v>14</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B46" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="C46" t="s">
         <v>11</v>
       </c>
       <c r="D46" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E46"/>
       <c r="F46"/>
@@ -1549,13 +1549,13 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" t="s">
+        <v>17</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B47" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="C47" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D47"/>
       <c r="E47">
@@ -1570,13 +1570,13 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" t="s">
+        <v>20</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B48" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="C48" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D48"/>
       <c r="E48">
@@ -1591,13 +1591,13 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" t="s">
+        <v>22</v>
+      </c>
+      <c r="B49" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B49" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="C49" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D49"/>
       <c r="E49">
@@ -1612,13 +1612,13 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
+        <v>24</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="C50" t="s">
         <v>26</v>
-      </c>
-      <c r="C50" t="s">
-        <v>27</v>
       </c>
       <c r="D50"/>
       <c r="E50"/>
@@ -1627,13 +1627,13 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
+        <v>27</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B51" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="C51" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D51"/>
       <c r="E51">
@@ -1657,7 +1657,7 @@
         <v>11</v>
       </c>
       <c r="D52" t="s">
-        <v>12</v>
+        <v>94</v>
       </c>
       <c r="E52"/>
       <c r="F52"/>
@@ -1665,16 +1665,16 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B53" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="C53" t="s">
         <v>11</v>
       </c>
       <c r="D53" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E53"/>
       <c r="F53"/>
@@ -1682,16 +1682,16 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" t="s">
+        <v>14</v>
+      </c>
+      <c r="B54" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B54" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="C54" t="s">
         <v>11</v>
       </c>
       <c r="D54" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E54"/>
       <c r="F54"/>
@@ -1699,13 +1699,13 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" t="s">
+        <v>17</v>
+      </c>
+      <c r="B55" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B55" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="C55" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D55"/>
       <c r="E55">
@@ -1720,13 +1720,13 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="s">
+        <v>20</v>
+      </c>
+      <c r="B56" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B56" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="C56" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D56"/>
       <c r="E56">
@@ -1741,13 +1741,13 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57" t="s">
+        <v>22</v>
+      </c>
+      <c r="B57" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B57" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="C57" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D57"/>
       <c r="E57">
@@ -1762,13 +1762,13 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58" t="s">
+        <v>24</v>
+      </c>
+      <c r="B58" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="C58" t="s">
         <v>26</v>
-      </c>
-      <c r="C58" t="s">
-        <v>27</v>
       </c>
       <c r="D58"/>
       <c r="E58"/>
@@ -1777,13 +1777,13 @@
     </row>
     <row r="59" spans="1:7">
       <c r="A59" t="s">
+        <v>27</v>
+      </c>
+      <c r="B59" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B59" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="C59" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D59"/>
       <c r="E59">
@@ -1807,7 +1807,7 @@
         <v>11</v>
       </c>
       <c r="D60" t="s">
-        <v>12</v>
+        <v>94</v>
       </c>
       <c r="E60"/>
       <c r="F60"/>
@@ -1815,16 +1815,16 @@
     </row>
     <row r="61" spans="1:7">
       <c r="A61" t="s">
+        <v>12</v>
+      </c>
+      <c r="B61" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B61" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="C61" t="s">
         <v>11</v>
       </c>
       <c r="D61" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E61"/>
       <c r="F61"/>
@@ -1832,16 +1832,16 @@
     </row>
     <row r="62" spans="1:7">
       <c r="A62" t="s">
+        <v>14</v>
+      </c>
+      <c r="B62" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B62" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="C62" t="s">
         <v>11</v>
       </c>
       <c r="D62" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E62"/>
       <c r="F62"/>
@@ -1849,13 +1849,13 @@
     </row>
     <row r="63" spans="1:7">
       <c r="A63" t="s">
+        <v>17</v>
+      </c>
+      <c r="B63" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B63" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="C63" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D63"/>
       <c r="E63">
@@ -1870,13 +1870,13 @@
     </row>
     <row r="64" spans="1:7">
       <c r="A64" t="s">
+        <v>20</v>
+      </c>
+      <c r="B64" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B64" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="C64" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D64"/>
       <c r="E64">
@@ -1891,13 +1891,13 @@
     </row>
     <row r="65" spans="1:7">
       <c r="A65" t="s">
+        <v>22</v>
+      </c>
+      <c r="B65" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B65" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="C65" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D65"/>
       <c r="E65">
@@ -1912,13 +1912,13 @@
     </row>
     <row r="66" spans="1:7">
       <c r="A66" t="s">
+        <v>24</v>
+      </c>
+      <c r="B66" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="C66" t="s">
         <v>26</v>
-      </c>
-      <c r="C66" t="s">
-        <v>27</v>
       </c>
       <c r="D66"/>
       <c r="E66"/>
@@ -1927,13 +1927,13 @@
     </row>
     <row r="67" spans="1:7">
       <c r="A67" t="s">
+        <v>27</v>
+      </c>
+      <c r="B67" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B67" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="C67" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D67"/>
       <c r="E67">
@@ -1957,7 +1957,7 @@
         <v>11</v>
       </c>
       <c r="D68" t="s">
-        <v>12</v>
+        <v>94</v>
       </c>
       <c r="E68"/>
       <c r="F68"/>
@@ -1965,16 +1965,16 @@
     </row>
     <row r="69" spans="1:7">
       <c r="A69" t="s">
+        <v>12</v>
+      </c>
+      <c r="B69" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B69" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="C69" t="s">
         <v>11</v>
       </c>
       <c r="D69" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E69"/>
       <c r="F69"/>
@@ -1982,16 +1982,16 @@
     </row>
     <row r="70" spans="1:7">
       <c r="A70" t="s">
+        <v>14</v>
+      </c>
+      <c r="B70" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B70" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="C70" t="s">
         <v>11</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E70"/>
       <c r="F70"/>
@@ -1999,13 +1999,13 @@
     </row>
     <row r="71" spans="1:7">
       <c r="A71" t="s">
+        <v>17</v>
+      </c>
+      <c r="B71" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B71" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="C71" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D71"/>
       <c r="E71">
@@ -2020,13 +2020,13 @@
     </row>
     <row r="72" spans="1:7">
       <c r="A72" t="s">
+        <v>20</v>
+      </c>
+      <c r="B72" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B72" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="C72" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D72"/>
       <c r="E72">
@@ -2041,13 +2041,13 @@
     </row>
     <row r="73" spans="1:7">
       <c r="A73" t="s">
+        <v>22</v>
+      </c>
+      <c r="B73" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B73" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="C73" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D73"/>
       <c r="E73">
@@ -2062,13 +2062,13 @@
     </row>
     <row r="74" spans="1:7">
       <c r="A74" t="s">
+        <v>24</v>
+      </c>
+      <c r="B74" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="C74" t="s">
         <v>26</v>
-      </c>
-      <c r="C74" t="s">
-        <v>27</v>
       </c>
       <c r="D74"/>
       <c r="E74"/>
@@ -2077,13 +2077,13 @@
     </row>
     <row r="75" spans="1:7">
       <c r="A75" t="s">
+        <v>27</v>
+      </c>
+      <c r="B75" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B75" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="C75" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D75"/>
       <c r="E75">
@@ -2107,7 +2107,7 @@
         <v>11</v>
       </c>
       <c r="D76" t="s">
-        <v>12</v>
+        <v>94</v>
       </c>
       <c r="E76"/>
       <c r="F76"/>
@@ -2115,16 +2115,16 @@
     </row>
     <row r="77" spans="1:7">
       <c r="A77" t="s">
+        <v>12</v>
+      </c>
+      <c r="B77" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B77" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="C77" t="s">
         <v>11</v>
       </c>
       <c r="D77" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E77"/>
       <c r="F77"/>
@@ -2132,16 +2132,16 @@
     </row>
     <row r="78" spans="1:7">
       <c r="A78" t="s">
+        <v>14</v>
+      </c>
+      <c r="B78" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B78" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="C78" t="s">
         <v>11</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E78"/>
       <c r="F78"/>
@@ -2149,13 +2149,13 @@
     </row>
     <row r="79" spans="1:7">
       <c r="A79" t="s">
+        <v>17</v>
+      </c>
+      <c r="B79" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B79" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="C79" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D79"/>
       <c r="E79">
@@ -2170,13 +2170,13 @@
     </row>
     <row r="80" spans="1:7">
       <c r="A80" t="s">
+        <v>20</v>
+      </c>
+      <c r="B80" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B80" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="C80" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D80"/>
       <c r="E80">
@@ -2191,13 +2191,13 @@
     </row>
     <row r="81" spans="1:7">
       <c r="A81" t="s">
+        <v>22</v>
+      </c>
+      <c r="B81" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B81" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="C81" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D81"/>
       <c r="E81">
@@ -2212,13 +2212,13 @@
     </row>
     <row r="82" spans="1:7">
       <c r="A82" t="s">
+        <v>24</v>
+      </c>
+      <c r="B82" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B82" s="3" t="s">
+      <c r="C82" t="s">
         <v>26</v>
-      </c>
-      <c r="C82" t="s">
-        <v>27</v>
       </c>
       <c r="D82"/>
       <c r="E82"/>
@@ -2227,13 +2227,13 @@
     </row>
     <row r="83" spans="1:7">
       <c r="A83" t="s">
+        <v>27</v>
+      </c>
+      <c r="B83" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B83" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="C83" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D83"/>
       <c r="E83">
@@ -2257,7 +2257,7 @@
         <v>11</v>
       </c>
       <c r="D84" t="s">
-        <v>12</v>
+        <v>94</v>
       </c>
       <c r="E84"/>
       <c r="F84"/>
@@ -2265,16 +2265,16 @@
     </row>
     <row r="85" spans="1:7">
       <c r="A85" t="s">
+        <v>12</v>
+      </c>
+      <c r="B85" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B85" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="C85" t="s">
         <v>11</v>
       </c>
       <c r="D85" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E85"/>
       <c r="F85"/>
@@ -2282,16 +2282,16 @@
     </row>
     <row r="86" spans="1:7">
       <c r="A86" t="s">
+        <v>14</v>
+      </c>
+      <c r="B86" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B86" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="C86" t="s">
         <v>11</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E86"/>
       <c r="F86"/>
@@ -2299,13 +2299,13 @@
     </row>
     <row r="87" spans="1:7">
       <c r="A87" t="s">
+        <v>17</v>
+      </c>
+      <c r="B87" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B87" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="C87" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D87"/>
       <c r="E87">
@@ -2320,13 +2320,13 @@
     </row>
     <row r="88" spans="1:7">
       <c r="A88" t="s">
+        <v>20</v>
+      </c>
+      <c r="B88" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B88" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="C88" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D88"/>
       <c r="E88">
@@ -2341,13 +2341,13 @@
     </row>
     <row r="89" spans="1:7">
       <c r="A89" t="s">
+        <v>22</v>
+      </c>
+      <c r="B89" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B89" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="C89" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D89"/>
       <c r="E89">
@@ -2362,13 +2362,13 @@
     </row>
     <row r="90" spans="1:7">
       <c r="A90" t="s">
+        <v>24</v>
+      </c>
+      <c r="B90" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B90" s="3" t="s">
+      <c r="C90" t="s">
         <v>26</v>
-      </c>
-      <c r="C90" t="s">
-        <v>27</v>
       </c>
       <c r="D90"/>
       <c r="E90"/>
@@ -2377,13 +2377,13 @@
     </row>
     <row r="91" spans="1:7">
       <c r="A91" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F91" s="5">
         <v>1</v>
@@ -2394,16 +2394,16 @@
     </row>
     <row r="92" spans="1:7">
       <c r="A92" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D92" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="B92" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C92" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D92" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="F92" s="5">
         <v>1</v>
@@ -2414,13 +2414,13 @@
     </row>
     <row r="93" spans="1:7" ht="30">
       <c r="A93" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C93" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E93">
         <v>1</v>
@@ -2434,13 +2434,13 @@
     </row>
     <row r="94" spans="1:7" ht="30">
       <c r="A94" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E94" s="5">
         <v>1</v>
@@ -2454,27 +2454,27 @@
     </row>
     <row r="95" spans="1:7">
       <c r="A95" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C95" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="30">
       <c r="A96" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E96" s="5">
         <v>1</v>
@@ -2488,13 +2488,13 @@
     </row>
     <row r="97" spans="1:7">
       <c r="A97" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E97" s="5">
         <v>1</v>
@@ -2508,13 +2508,13 @@
     </row>
     <row r="98" spans="1:7">
       <c r="A98" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E98" s="5">
         <v>1</v>
@@ -2528,13 +2528,13 @@
     </row>
     <row r="99" spans="1:7" ht="30">
       <c r="A99" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E99" s="5">
         <v>1</v>
@@ -2548,13 +2548,13 @@
     </row>
     <row r="100" spans="1:7">
       <c r="A100" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E100" s="5">
         <v>1</v>
@@ -2568,38 +2568,38 @@
     </row>
     <row r="101" spans="1:7">
       <c r="A101" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="102" spans="1:7">
       <c r="A102" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C102" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="30">
       <c r="A103" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E103" s="5">
         <v>1</v>
@@ -2613,13 +2613,13 @@
     </row>
     <row r="104" spans="1:7">
       <c r="A104" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E104" s="5">
         <v>1</v>
@@ -2633,13 +2633,13 @@
     </row>
     <row r="105" spans="1:7">
       <c r="A105" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C105" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E105" s="5">
         <v>1</v>
@@ -2653,13 +2653,13 @@
     </row>
     <row r="106" spans="1:7" ht="30">
       <c r="A106" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E106" s="5">
         <v>1</v>
@@ -2673,13 +2673,13 @@
     </row>
     <row r="107" spans="1:7">
       <c r="A107" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C107" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E107" s="5">
         <v>1</v>
@@ -2693,38 +2693,38 @@
     </row>
     <row r="108" spans="1:7">
       <c r="A108" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C108" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="109" spans="1:7">
       <c r="A109" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C109" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D109" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="110" spans="1:7" ht="30">
       <c r="A110" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C110" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E110" s="5">
         <v>1</v>
@@ -2738,13 +2738,13 @@
     </row>
     <row r="111" spans="1:7">
       <c r="A111" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C111" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E111" s="5">
         <v>1</v>
@@ -2758,13 +2758,13 @@
     </row>
     <row r="112" spans="1:7">
       <c r="A112" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C112" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E112" s="5">
         <v>1</v>
@@ -2778,13 +2778,13 @@
     </row>
     <row r="113" spans="1:7" ht="30">
       <c r="A113" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C113" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E113" s="5">
         <v>1</v>
@@ -2798,13 +2798,13 @@
     </row>
     <row r="114" spans="1:7">
       <c r="A114" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E114" s="5">
         <v>1</v>
@@ -2818,38 +2818,38 @@
     </row>
     <row r="115" spans="1:7">
       <c r="A115" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C115" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="116" spans="1:7">
       <c r="A116" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C116" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D116" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="117" spans="1:7" ht="30">
       <c r="A117" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C117" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E117" s="5">
         <v>1</v>
@@ -2863,13 +2863,13 @@
     </row>
     <row r="118" spans="1:7">
       <c r="A118" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E118" s="5">
         <v>1</v>
@@ -2883,13 +2883,13 @@
     </row>
     <row r="119" spans="1:7">
       <c r="A119" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E119" s="5">
         <v>1</v>
@@ -2903,13 +2903,13 @@
     </row>
     <row r="120" spans="1:7" ht="30">
       <c r="A120" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E120" s="5">
         <v>1</v>
@@ -2923,13 +2923,13 @@
     </row>
     <row r="121" spans="1:7">
       <c r="A121" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C121" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E121" s="5">
         <v>1</v>
@@ -2943,38 +2943,38 @@
     </row>
     <row r="122" spans="1:7">
       <c r="A122" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C122" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="123" spans="1:7">
       <c r="A123" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C123" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D123" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="124" spans="1:7" ht="30">
       <c r="A124" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C124" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E124" s="5">
         <v>1</v>
@@ -2988,13 +2988,13 @@
     </row>
     <row r="125" spans="1:7">
       <c r="A125" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C125" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E125" s="5">
         <v>1</v>
@@ -3008,13 +3008,13 @@
     </row>
     <row r="126" spans="1:7">
       <c r="A126" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C126" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E126" s="5">
         <v>1</v>
@@ -3028,13 +3028,13 @@
     </row>
     <row r="127" spans="1:7" ht="30">
       <c r="A127" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C127" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E127" s="5">
         <v>1</v>
@@ -3048,13 +3048,13 @@
     </row>
     <row r="128" spans="1:7">
       <c r="A128" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C128" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E128" s="5">
         <v>1</v>
@@ -3068,38 +3068,38 @@
     </row>
     <row r="129" spans="1:7">
       <c r="A129" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C129" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="130" spans="1:7">
       <c r="A130" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B130" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C130" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D130" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="B130" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C130" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D130" s="5" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="131" spans="1:7" ht="30">
       <c r="A131" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C131" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E131" s="5">
         <v>1</v>
@@ -3113,13 +3113,13 @@
     </row>
     <row r="132" spans="1:7">
       <c r="A132" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C132" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E132" s="5">
         <v>1</v>
@@ -3133,13 +3133,13 @@
     </row>
     <row r="133" spans="1:7">
       <c r="A133" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C133" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E133" s="5">
         <v>1</v>
@@ -3153,13 +3153,13 @@
     </row>
     <row r="134" spans="1:7" ht="30">
       <c r="A134" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C134" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E134" s="5">
         <v>1</v>
@@ -3173,13 +3173,13 @@
     </row>
     <row r="135" spans="1:7">
       <c r="A135" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C135" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E135" s="5">
         <v>1</v>
@@ -3193,38 +3193,38 @@
     </row>
     <row r="136" spans="1:7">
       <c r="A136" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C136" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="137" spans="1:7">
       <c r="A137" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C137" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D137" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="138" spans="1:7" ht="30">
       <c r="A138" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C138" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E138" s="5">
         <v>1</v>
@@ -3238,13 +3238,13 @@
     </row>
     <row r="139" spans="1:7">
       <c r="A139" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C139" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E139" s="5">
         <v>1</v>
@@ -3258,13 +3258,13 @@
     </row>
     <row r="140" spans="1:7">
       <c r="A140" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B140" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C140" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E140" s="5">
         <v>1</v>
@@ -3278,13 +3278,13 @@
     </row>
     <row r="141" spans="1:7" ht="30">
       <c r="A141" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C141" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E141" s="5">
         <v>1</v>
@@ -3298,13 +3298,13 @@
     </row>
     <row r="142" spans="1:7">
       <c r="A142" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B142" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C142" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E142" s="5">
         <v>1</v>
@@ -3318,38 +3318,38 @@
     </row>
     <row r="143" spans="1:7">
       <c r="A143" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C143" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="144" spans="1:7">
       <c r="A144" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C144" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D144" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="145" spans="1:7" ht="30">
       <c r="A145" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B145" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C145" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E145" s="5">
         <v>1</v>
@@ -3363,13 +3363,13 @@
     </row>
     <row r="146" spans="1:7">
       <c r="A146" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C146" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E146" s="5">
         <v>1</v>
@@ -3383,13 +3383,13 @@
     </row>
     <row r="147" spans="1:7">
       <c r="A147" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C147" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E147" s="5">
         <v>1</v>
@@ -3403,13 +3403,13 @@
     </row>
     <row r="148" spans="1:7" ht="30">
       <c r="A148" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C148" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E148" s="5">
         <v>1</v>
@@ -3423,13 +3423,13 @@
     </row>
     <row r="149" spans="1:7">
       <c r="A149" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B149" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C149" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E149" s="5">
         <v>1</v>
@@ -3443,38 +3443,38 @@
     </row>
     <row r="150" spans="1:7">
       <c r="A150" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B150" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C150" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="151" spans="1:7">
       <c r="A151" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B151" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C151" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D151" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="152" spans="1:7" ht="30">
       <c r="A152" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C152" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E152" s="5">
         <v>1</v>
@@ -3488,13 +3488,13 @@
     </row>
     <row r="153" spans="1:7">
       <c r="A153" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C153" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E153" s="5">
         <v>1</v>
@@ -3508,13 +3508,13 @@
     </row>
     <row r="154" spans="1:7">
       <c r="A154" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B154" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C154" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E154" s="5">
         <v>1</v>
@@ -3528,13 +3528,13 @@
     </row>
     <row r="155" spans="1:7" ht="30">
       <c r="A155" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B155" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C155" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E155" s="5">
         <v>1</v>
@@ -3548,13 +3548,13 @@
     </row>
     <row r="156" spans="1:7">
       <c r="A156" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C156" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E156" s="5">
         <v>1</v>
@@ -3568,38 +3568,38 @@
     </row>
     <row r="157" spans="1:7">
       <c r="A157" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B157" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C157" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="158" spans="1:7">
       <c r="A158" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B158" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C158" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D158" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="159" spans="1:7" ht="30">
       <c r="A159" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B159" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C159" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E159" s="5">
         <v>1</v>
@@ -3613,13 +3613,13 @@
     </row>
     <row r="160" spans="1:7">
       <c r="A160" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B160" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C160" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E160" s="5">
         <v>1</v>
@@ -3633,13 +3633,13 @@
     </row>
     <row r="161" spans="1:7">
       <c r="A161" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B161" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C161" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E161" s="5">
         <v>1</v>
@@ -3653,13 +3653,13 @@
     </row>
     <row r="162" spans="1:7" ht="30">
       <c r="A162" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B162" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C162" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E162" s="5">
         <v>1</v>
@@ -3673,13 +3673,13 @@
     </row>
     <row r="163" spans="1:7">
       <c r="A163" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B163" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C163" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E163" s="5">
         <v>1</v>
@@ -3693,13 +3693,13 @@
     </row>
     <row r="164" spans="1:7">
       <c r="A164" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B164" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C164" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>